<commit_message>
:art: Barplot graph added for better visualization of each dataset
</commit_message>
<xml_diff>
--- a/EmploymentRates/employment_rate_citizenship_clean.xlsx
+++ b/EmploymentRates/employment_rate_citizenship_clean.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\teomeo\Desktop\aYEAR4\semester 2\Data Analysis\DPII\EmploymentRates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D5D9E25-C678-4841-8FA3-571971462106}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EC21581-5BD9-4EA0-ACBD-5D24424AC491}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{CF552007-EEB0-42EA-9496-7702210DC9AE}"/>
+    <workbookView xWindow="3624" yWindow="1572" windowWidth="24372" windowHeight="14628" xr2:uid="{CF552007-EEB0-42EA-9496-7702210DC9AE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1022" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1021" uniqueCount="66">
   <si>
     <t>2000</t>
   </si>
@@ -697,8 +697,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCC36C11-C521-4BC8-98A1-5DDF7C2F0C6A}">
   <dimension ref="A1:AU36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="AP29" sqref="AP29"/>
+    <sheetView tabSelected="1" topLeftCell="Y7" workbookViewId="0">
+      <selection activeCell="AO39" sqref="AO39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5400,8 +5400,8 @@
       <c r="AM33" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="AN33" s="3" t="s">
-        <v>27</v>
+      <c r="AN33" s="3">
+        <v>60</v>
       </c>
       <c r="AO33" s="3" t="s">
         <v>1</v>
@@ -5856,6 +5856,21 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="N1:O1"/>
+    <mergeCell ref="P1:Q1"/>
+    <mergeCell ref="R1:S1"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="V1:W1"/>
+    <mergeCell ref="X1:Y1"/>
+    <mergeCell ref="Z1:AA1"/>
+    <mergeCell ref="AB1:AC1"/>
+    <mergeCell ref="AD1:AE1"/>
     <mergeCell ref="AP1:AQ1"/>
     <mergeCell ref="AR1:AS1"/>
     <mergeCell ref="AT1:AU1"/>
@@ -5864,21 +5879,6 @@
     <mergeCell ref="AJ1:AK1"/>
     <mergeCell ref="AL1:AM1"/>
     <mergeCell ref="AN1:AO1"/>
-    <mergeCell ref="V1:W1"/>
-    <mergeCell ref="X1:Y1"/>
-    <mergeCell ref="Z1:AA1"/>
-    <mergeCell ref="AB1:AC1"/>
-    <mergeCell ref="AD1:AE1"/>
-    <mergeCell ref="L1:M1"/>
-    <mergeCell ref="N1:O1"/>
-    <mergeCell ref="P1:Q1"/>
-    <mergeCell ref="R1:S1"/>
-    <mergeCell ref="T1:U1"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="J1:K1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>